<commit_message>
👌 IMPROVE: Updated and added all points per dollar
</commit_message>
<xml_diff>
--- a/2020_prflplayers.xlsx
+++ b/2020_prflplayers.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GIT\prfl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854F632A-D5F6-46C6-A2C7-7DCFBFB86E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA733FF-E5F9-49FC-83B8-B0F22B60B110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{BA228D13-2244-495E-B498-5A53B12CE2AB}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{68C4CD1C-F6FC-42D1-9C86-4B42BFFB4529}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{68C4CD1C-F6FC-42D1-9C86-4B42BFFB4529}"/>
   </bookViews>
   <sheets>
     <sheet name="QB" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8081" uniqueCount="3093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8090" uniqueCount="3093">
   <si>
     <t>#</t>
   </si>
@@ -10707,8 +10707,8 @@
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AC1" sqref="AC1:AO7"/>
     </sheetView>
-    <sheetView topLeftCell="P1" workbookViewId="1">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="1">
+      <selection activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11706,6 +11706,52 @@
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>464.17333333333335</v>
       </c>
+      <c r="AC9" t="s">
+        <v>2355</v>
+      </c>
+      <c r="AD9">
+        <f>AVERAGE(AA2:AA65)</f>
+        <v>128.72178575828019</v>
+      </c>
+      <c r="AE9">
+        <f>AVERAGE(AA2:AA33)</f>
+        <v>254.71121741933729</v>
+      </c>
+      <c r="AF9">
+        <f>AVERAGE(AA2:AA17)</f>
+        <v>222.5749772652116</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>2356</v>
+      </c>
+      <c r="AI9">
+        <f>AD9-(3*AD10)</f>
+        <v>-581.6278218061841</v>
+      </c>
+      <c r="AJ9">
+        <f>AD9-(2*AD10)</f>
+        <v>-344.84461928469608</v>
+      </c>
+      <c r="AK9">
+        <f>AD9-(AD10)</f>
+        <v>-108.06141676320794</v>
+      </c>
+      <c r="AL9">
+        <f>AD9</f>
+        <v>128.72178575828019</v>
+      </c>
+      <c r="AM9">
+        <f>AD9+AD10</f>
+        <v>365.50498827976833</v>
+      </c>
+      <c r="AN9">
+        <f>AD9+(2*AD10)</f>
+        <v>602.28819080125641</v>
+      </c>
+      <c r="AO9">
+        <f>AD9+(3*AD10)</f>
+        <v>839.0713933227446</v>
+      </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -11785,6 +11831,52 @@
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>12.19814814814815</v>
       </c>
+      <c r="AC10" t="s">
+        <v>2359</v>
+      </c>
+      <c r="AD10">
+        <f>_xlfn.STDEV.P(AA2:AA65)</f>
+        <v>236.78320252148814</v>
+      </c>
+      <c r="AE10">
+        <f>_xlfn.STDEV.P(AA2:AA33)</f>
+        <v>283.13706784821295</v>
+      </c>
+      <c r="AF10">
+        <f>_xlfn.STDEV.P(AA2:AA17)</f>
+        <v>302.18651869188687</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>2357</v>
+      </c>
+      <c r="AI10">
+        <f>AE9-(3*AE10)</f>
+        <v>-594.69998612530162</v>
+      </c>
+      <c r="AJ10">
+        <f>AE9-(2*AE10)</f>
+        <v>-311.56291827708861</v>
+      </c>
+      <c r="AK10">
+        <f>AE9-AE10</f>
+        <v>-28.425850428875663</v>
+      </c>
+      <c r="AL10">
+        <f>AE9</f>
+        <v>254.71121741933729</v>
+      </c>
+      <c r="AM10">
+        <f>AE9+AE10</f>
+        <v>537.84828526755018</v>
+      </c>
+      <c r="AN10">
+        <f>AE9+(2*AE10)</f>
+        <v>820.98535311576325</v>
+      </c>
+      <c r="AO10">
+        <f>AE9+(3*AE10)</f>
+        <v>1104.1224209639761</v>
+      </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -11864,6 +11956,52 @@
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>1248.72</v>
       </c>
+      <c r="AC11" t="s">
+        <v>2360</v>
+      </c>
+      <c r="AD11">
+        <f>_xlfn.VAR.P(AA2:AA65)</f>
+        <v>56066.284996332062</v>
+      </c>
+      <c r="AE11">
+        <f>_xlfn.VAR.P(AA2:AA33)</f>
+        <v>80166.599189683548</v>
+      </c>
+      <c r="AF11">
+        <f>_xlfn.VAR.P(AA2:AA17)</f>
+        <v>91316.692079122091</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>2358</v>
+      </c>
+      <c r="AI11">
+        <f>AF9-(3*AF10)</f>
+        <v>-683.98457881044897</v>
+      </c>
+      <c r="AJ11">
+        <f>AF9-(2*AF10)</f>
+        <v>-381.79806011856215</v>
+      </c>
+      <c r="AK11">
+        <f>AF9-AF10</f>
+        <v>-79.611541426675274</v>
+      </c>
+      <c r="AL11">
+        <f>AF9</f>
+        <v>222.5749772652116</v>
+      </c>
+      <c r="AM11">
+        <f>AF9+AF10</f>
+        <v>524.76149595709853</v>
+      </c>
+      <c r="AN11">
+        <f>AF9+(2*AF10)</f>
+        <v>826.94801464898535</v>
+      </c>
+      <c r="AO11">
+        <f>AF9+(3*AF10)</f>
+        <v>1129.1345333408722</v>
+      </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -11943,6 +12081,37 @@
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>286.91000000000003</v>
       </c>
+      <c r="AH12" t="s">
+        <v>2356</v>
+      </c>
+      <c r="AI12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AI9)</f>
+        <v>64</v>
+      </c>
+      <c r="AJ12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AJ9)</f>
+        <v>64</v>
+      </c>
+      <c r="AK12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AK9)</f>
+        <v>64</v>
+      </c>
+      <c r="AL12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AL9)</f>
+        <v>19</v>
+      </c>
+      <c r="AM12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AM9)</f>
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AN9)</f>
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <f>COUNTIF(C9:C72,"&gt;" &amp; AO9)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -12022,6 +12191,37 @@
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>130.565</v>
       </c>
+      <c r="AH13" t="s">
+        <v>2357</v>
+      </c>
+      <c r="AI13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AI10)</f>
+        <v>32</v>
+      </c>
+      <c r="AJ13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AJ10)</f>
+        <v>32</v>
+      </c>
+      <c r="AK13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AK10)</f>
+        <v>32</v>
+      </c>
+      <c r="AL13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AL10)</f>
+        <v>5</v>
+      </c>
+      <c r="AM13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AM10)</f>
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AN10)</f>
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <f>COUNTIF(C9:C40,"&gt;" &amp; AO10)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -12100,6 +12300,37 @@
       <c r="AA14">
         <f>Table_1[[#This Row],[Pts]]/Table_1[[#This Row],[Salary]]</f>
         <v>503.7</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>2358</v>
+      </c>
+      <c r="AI14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AI11)</f>
+        <v>16</v>
+      </c>
+      <c r="AJ14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AJ11)</f>
+        <v>16</v>
+      </c>
+      <c r="AK14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AK11)</f>
+        <v>16</v>
+      </c>
+      <c r="AL14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AL11)</f>
+        <v>9</v>
+      </c>
+      <c r="AM14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AM11)</f>
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AN11)</f>
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <f>COUNTIF(C9:C24,"&gt;" &amp; AO11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -58165,7 +58396,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:U143"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="1">
+    <sheetView topLeftCell="J1" workbookViewId="1">
       <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>

</xml_diff>